<commit_message>
Create new project used for prototyping and consumption measurement.
</commit_message>
<xml_diff>
--- a/doc/MotionModule-PowerConsumption.xlsx
+++ b/doc/MotionModule-PowerConsumption.xlsx
@@ -4,21 +4,27 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Ideal" sheetId="1" r:id="rId1"/>
+    <sheet name="Reality-Inactive" sheetId="2" r:id="rId2"/>
+    <sheet name="Reality-Active" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="AVG_CURRENT">Sheet1!$F$8</definedName>
-    <definedName name="PERIOD">Sheet1!$C$8</definedName>
+    <definedName name="AVG_CURRENT" localSheetId="2">'Reality-Active'!$F$8</definedName>
+    <definedName name="AVG_CURRENT" localSheetId="1">'Reality-Inactive'!$F$7</definedName>
+    <definedName name="AVG_CURRENT">Ideal!$F$8</definedName>
+    <definedName name="PERIOD" localSheetId="2">'Reality-Active'!$C$8</definedName>
+    <definedName name="PERIOD" localSheetId="1">'Reality-Inactive'!$C$7</definedName>
+    <definedName name="PERIOD">Ideal!$C$8</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="36">
   <si>
     <t>Activity</t>
   </si>
@@ -109,6 +115,25 @@
   </si>
   <si>
     <t>PIR sensor 50u static (90% time)</t>
+  </si>
+  <si>
+    <t>NRF powerup</t>
+  </si>
+  <si>
+    <t>Duration ms</t>
+  </si>
+  <si>
+    <t>NRF powered up only for transmissions. Powerup time is 100 ms. Consumption measured 1.5mA</t>
+  </si>
+  <si>
+    <t>Execution period s</t>
+  </si>
+  <si>
+    <t>Idle+PIR static</t>
+  </si>
+  <si>
+    <t>PWR_DWN; ADC,WDT,BOD enabled. 
+MCU: 5uA. PIR: 50u</t>
   </si>
 </sst>
 </file>
@@ -253,7 +278,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -284,6 +309,105 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -590,7 +714,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
@@ -642,7 +766,7 @@
         <v>30</v>
       </c>
       <c r="E2" s="5">
-        <f t="shared" ref="E2:E4" si="0">B2/C2/1000</f>
+        <f t="shared" ref="E2:E3" si="0">B2/C2/1000</f>
         <v>4.0000000000000002E-4</v>
       </c>
       <c r="F2" s="17">
@@ -912,4 +1036,659 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12" style="50" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" style="50" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.6640625" style="50" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.6640625" style="50" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.88671875" style="50" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.5546875" style="50" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="46" style="32" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="33" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="34" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" s="35" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" s="34" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="35" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="34" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="28" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="36" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="37">
+        <v>2</v>
+      </c>
+      <c r="C2" s="38">
+        <v>10</v>
+      </c>
+      <c r="D2" s="39">
+        <v>30</v>
+      </c>
+      <c r="E2" s="40">
+        <f>B2/C2/1000</f>
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="F2" s="41">
+        <f t="shared" ref="F2:F5" si="0">D2*E2</f>
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="G2" s="29" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="36" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="37">
+        <v>2</v>
+      </c>
+      <c r="C3" s="38">
+        <v>60</v>
+      </c>
+      <c r="D3" s="39">
+        <v>30</v>
+      </c>
+      <c r="E3" s="40">
+        <f>B3/C3/1000</f>
+        <v>3.3333333333333335E-5</v>
+      </c>
+      <c r="F3" s="41">
+        <f t="shared" si="0"/>
+        <v>1E-3</v>
+      </c>
+      <c r="G3" s="29" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="36" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" s="37">
+        <v>100</v>
+      </c>
+      <c r="C4" s="38">
+        <v>10</v>
+      </c>
+      <c r="D4" s="42">
+        <v>1.5</v>
+      </c>
+      <c r="E4" s="40">
+        <f>B4/C4/1000</f>
+        <v>0.01</v>
+      </c>
+      <c r="F4" s="41">
+        <f t="shared" si="0"/>
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="G4" s="29" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="36" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="37"/>
+      <c r="C5" s="38"/>
+      <c r="D5" s="39">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="E5" s="40">
+        <f>1 -SUM(E2:E4)</f>
+        <v>0.98976666666666668</v>
+      </c>
+      <c r="F5" s="41">
+        <f t="shared" si="0"/>
+        <v>4.9488333333333337E-3</v>
+      </c>
+      <c r="G5" s="29" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="36"/>
+      <c r="B6" s="39"/>
+      <c r="C6" s="38"/>
+      <c r="D6" s="39"/>
+      <c r="E6" s="38"/>
+      <c r="F6" s="39"/>
+      <c r="G6" s="29"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="43" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="44"/>
+      <c r="C7" s="45"/>
+      <c r="D7" s="44"/>
+      <c r="E7" s="46">
+        <f>SUM(E2:E5)</f>
+        <v>1</v>
+      </c>
+      <c r="F7" s="47">
+        <f>SUM(F2:F5)</f>
+        <v>2.6948833333333332E-2</v>
+      </c>
+      <c r="G7" s="30"/>
+    </row>
+    <row r="9" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="33" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="34" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="35" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" s="34" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" s="48"/>
+      <c r="F9" s="48"/>
+      <c r="G9" s="31"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" s="36" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="39">
+        <v>18</v>
+      </c>
+      <c r="C10" s="49">
+        <f t="shared" ref="C10:C17" si="1">B10/AVG_CURRENT</f>
+        <v>667.93243987061908</v>
+      </c>
+      <c r="D10" s="37">
+        <f>C10/24</f>
+        <v>27.83051832794246</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" s="36" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="39">
+        <v>68</v>
+      </c>
+      <c r="C11" s="49">
+        <f t="shared" si="1"/>
+        <v>2523.3003284001165</v>
+      </c>
+      <c r="D11" s="37">
+        <f t="shared" ref="D11:D17" si="2">C11/24</f>
+        <v>105.13751368333818</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" s="51" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="52">
+        <v>210</v>
+      </c>
+      <c r="C12" s="53">
+        <f t="shared" si="1"/>
+        <v>7792.5451318238893</v>
+      </c>
+      <c r="D12" s="54">
+        <f t="shared" si="2"/>
+        <v>324.68938049266205</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" s="36" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="39">
+        <v>900</v>
+      </c>
+      <c r="C13" s="49">
+        <f t="shared" si="1"/>
+        <v>33396.621993530956</v>
+      </c>
+      <c r="D13" s="37">
+        <f t="shared" si="2"/>
+        <v>1391.5259163971232</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" s="36" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" s="39">
+        <v>1250</v>
+      </c>
+      <c r="C14" s="49">
+        <f t="shared" si="1"/>
+        <v>46384.197213237436</v>
+      </c>
+      <c r="D14" s="37">
+        <f t="shared" si="2"/>
+        <v>1932.6748838848932</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" s="36" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" s="39">
+        <v>2400</v>
+      </c>
+      <c r="C15" s="49">
+        <f t="shared" si="1"/>
+        <v>89057.658649415869</v>
+      </c>
+      <c r="D15" s="37">
+        <f t="shared" si="2"/>
+        <v>3710.7357770589947</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" s="55" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" s="56">
+        <v>2890</v>
+      </c>
+      <c r="C16" s="57">
+        <f t="shared" si="1"/>
+        <v>107240.26395700495</v>
+      </c>
+      <c r="D16" s="58">
+        <f t="shared" si="2"/>
+        <v>4468.3443315418726</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="43" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17" s="44">
+        <v>4400</v>
+      </c>
+      <c r="C17" s="59">
+        <f t="shared" si="1"/>
+        <v>163272.37419059576</v>
+      </c>
+      <c r="D17" s="60">
+        <f t="shared" si="2"/>
+        <v>6803.0155912748232</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12.5546875" style="50" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" style="50" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.6640625" style="50" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.6640625" style="50" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.88671875" style="50" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.5546875" style="50" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="46" style="32" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="33" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="34" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" s="35" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" s="34" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="35" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="34" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="28" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="36" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="37">
+        <v>2</v>
+      </c>
+      <c r="C2" s="38">
+        <v>10</v>
+      </c>
+      <c r="D2" s="39">
+        <v>30</v>
+      </c>
+      <c r="E2" s="40">
+        <f>B2/C2/1000</f>
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="F2" s="41">
+        <f t="shared" ref="F2:F6" si="0">D2*E2</f>
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="G2" s="29" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="36" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="37">
+        <v>2</v>
+      </c>
+      <c r="C3" s="38">
+        <v>60</v>
+      </c>
+      <c r="D3" s="39">
+        <v>30</v>
+      </c>
+      <c r="E3" s="40">
+        <f>B3/C3/1000</f>
+        <v>3.3333333333333335E-5</v>
+      </c>
+      <c r="F3" s="41">
+        <f t="shared" si="0"/>
+        <v>1E-3</v>
+      </c>
+      <c r="G3" s="29" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="36" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" s="37">
+        <v>100</v>
+      </c>
+      <c r="C4" s="38">
+        <v>10</v>
+      </c>
+      <c r="D4" s="42">
+        <v>1.5</v>
+      </c>
+      <c r="E4" s="40">
+        <f>B4/C4/1000</f>
+        <v>0.01</v>
+      </c>
+      <c r="F4" s="41">
+        <f t="shared" si="0"/>
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="G4" s="29" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="36" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="37">
+        <v>0</v>
+      </c>
+      <c r="C5" s="38">
+        <v>86400</v>
+      </c>
+      <c r="D5" s="39">
+        <v>0.15</v>
+      </c>
+      <c r="E5" s="40">
+        <f>B5/C5/1000</f>
+        <v>0</v>
+      </c>
+      <c r="F5" s="41">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G5" s="29" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" s="37"/>
+      <c r="C6" s="38"/>
+      <c r="D6" s="39">
+        <v>5.5E-2</v>
+      </c>
+      <c r="E6" s="40">
+        <f>1 -SUM(E2:E5)</f>
+        <v>0.98976666666666668</v>
+      </c>
+      <c r="F6" s="41">
+        <f t="shared" si="0"/>
+        <v>5.4437166666666668E-2</v>
+      </c>
+      <c r="G6" s="29" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="36"/>
+      <c r="B7" s="39"/>
+      <c r="C7" s="38"/>
+      <c r="D7" s="39"/>
+      <c r="E7" s="38"/>
+      <c r="F7" s="39"/>
+      <c r="G7" s="29"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="43" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="44"/>
+      <c r="C8" s="45"/>
+      <c r="D8" s="44"/>
+      <c r="E8" s="46">
+        <f>SUM(E2:E6)</f>
+        <v>1</v>
+      </c>
+      <c r="F8" s="47">
+        <f>SUM(F2:F6)</f>
+        <v>7.6437166666666667E-2</v>
+      </c>
+      <c r="G8" s="30"/>
+    </row>
+    <row r="10" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="33" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="34" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="35" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" s="34" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" s="48"/>
+      <c r="F10" s="48"/>
+      <c r="G10" s="31"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" s="36" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="39">
+        <v>18</v>
+      </c>
+      <c r="C11" s="49">
+        <f t="shared" ref="C11:C18" si="1">B11/AVG_CURRENT</f>
+        <v>235.48753551391883</v>
+      </c>
+      <c r="D11" s="37">
+        <f>C11/24</f>
+        <v>9.8119806464132839</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" s="36" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="39">
+        <v>68</v>
+      </c>
+      <c r="C12" s="49">
+        <f t="shared" si="1"/>
+        <v>889.61957860813789</v>
+      </c>
+      <c r="D12" s="37">
+        <f t="shared" ref="D12:D18" si="2">C12/24</f>
+        <v>37.067482442005748</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" s="51" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="52">
+        <v>210</v>
+      </c>
+      <c r="C13" s="53">
+        <f t="shared" si="1"/>
+        <v>2747.35458099572</v>
+      </c>
+      <c r="D13" s="54">
+        <f t="shared" si="2"/>
+        <v>114.47310754148833</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" s="36" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="39">
+        <v>900</v>
+      </c>
+      <c r="C14" s="49">
+        <f t="shared" si="1"/>
+        <v>11774.376775695942</v>
+      </c>
+      <c r="D14" s="37">
+        <f t="shared" si="2"/>
+        <v>490.59903232066426</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" s="36" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" s="39">
+        <v>1250</v>
+      </c>
+      <c r="C15" s="49">
+        <f t="shared" si="1"/>
+        <v>16353.301077355474</v>
+      </c>
+      <c r="D15" s="37">
+        <f t="shared" si="2"/>
+        <v>681.38754488981147</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" s="36" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" s="39">
+        <v>2400</v>
+      </c>
+      <c r="C16" s="49">
+        <f t="shared" si="1"/>
+        <v>31398.338068522513</v>
+      </c>
+      <c r="D16" s="37">
+        <f t="shared" si="2"/>
+        <v>1308.2640861884381</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="55" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" s="56">
+        <v>2890</v>
+      </c>
+      <c r="C17" s="57">
+        <f t="shared" si="1"/>
+        <v>37808.832090845855</v>
+      </c>
+      <c r="D17" s="58">
+        <f t="shared" si="2"/>
+        <v>1575.3680037852439</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="43" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18" s="44">
+        <v>4400</v>
+      </c>
+      <c r="C18" s="59">
+        <f t="shared" si="1"/>
+        <v>57563.619792291269</v>
+      </c>
+      <c r="D18" s="60">
+        <f t="shared" si="2"/>
+        <v>2398.484158012136</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Compute consumption measurement of future motion module update (2 power cells). Update tasks list.
</commit_message>
<xml_diff>
--- a/doc/MotionModule-PowerConsumption.xlsx
+++ b/doc/MotionModule-PowerConsumption.xlsx
@@ -4,17 +4,23 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Ideal" sheetId="1" r:id="rId1"/>
     <sheet name="Reality-Inactive" sheetId="2" r:id="rId2"/>
     <sheet name="Reality-Active" sheetId="3" r:id="rId3"/>
+    <sheet name="MCU" sheetId="4" r:id="rId4"/>
+    <sheet name="PIR-Active" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
+    <definedName name="AVG_CURRENT" localSheetId="3">MCU!$F$8</definedName>
+    <definedName name="AVG_CURRENT" localSheetId="4">'PIR-Active'!$F$6</definedName>
     <definedName name="AVG_CURRENT" localSheetId="2">'Reality-Active'!$F$8</definedName>
     <definedName name="AVG_CURRENT" localSheetId="1">'Reality-Inactive'!$F$7</definedName>
     <definedName name="AVG_CURRENT">Ideal!$F$8</definedName>
+    <definedName name="PERIOD" localSheetId="3">MCU!$C$8</definedName>
+    <definedName name="PERIOD" localSheetId="4">'PIR-Active'!$C$6</definedName>
     <definedName name="PERIOD" localSheetId="2">'Reality-Active'!$C$8</definedName>
     <definedName name="PERIOD" localSheetId="1">'Reality-Inactive'!$C$7</definedName>
     <definedName name="PERIOD">Ideal!$C$8</definedName>
@@ -24,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="42">
   <si>
     <t>Activity</t>
   </si>
@@ -134,6 +140,24 @@
   <si>
     <t>PWR_DWN; ADC,WDT,BOD enabled. 
 MCU: 5uA. PIR: 50u</t>
+  </si>
+  <si>
+    <t>NRF</t>
+  </si>
+  <si>
+    <t>NRF active</t>
+  </si>
+  <si>
+    <t>No PIR</t>
+  </si>
+  <si>
+    <t>PIR sensor 50u static</t>
+  </si>
+  <si>
+    <t>PIR is off (alarm unlocked) most of the time</t>
+  </si>
+  <si>
+    <t>PIR sensor 150u during motion</t>
   </si>
 </sst>
 </file>
@@ -1042,7 +1066,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
@@ -1691,4 +1715,588 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="46" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="15">
+        <v>100</v>
+      </c>
+      <c r="C2" s="4">
+        <v>10000</v>
+      </c>
+      <c r="D2" s="13">
+        <v>3</v>
+      </c>
+      <c r="E2" s="5">
+        <f>B2/C2</f>
+        <v>0.01</v>
+      </c>
+      <c r="F2" s="17">
+        <f t="shared" ref="F2:F6" si="0">D2*E2</f>
+        <v>0.03</v>
+      </c>
+      <c r="G2" s="13"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" s="15">
+        <v>2</v>
+      </c>
+      <c r="C3" s="4">
+        <v>10000</v>
+      </c>
+      <c r="D3" s="13">
+        <v>20</v>
+      </c>
+      <c r="E3" s="5">
+        <f>B3/C3</f>
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="F3" s="17">
+        <f t="shared" si="0"/>
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="G3" s="13"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="2"/>
+      <c r="B4" s="15"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G4" s="23"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="2"/>
+      <c r="B5" s="15"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G5" s="23"/>
+    </row>
+    <row r="6" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="15"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="13">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="E6" s="5">
+        <f>1 -SUM(E2:E5)</f>
+        <v>0.98980000000000001</v>
+      </c>
+      <c r="F6" s="17">
+        <f t="shared" si="0"/>
+        <v>4.9490000000000003E-3</v>
+      </c>
+      <c r="G6" s="23" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="2"/>
+      <c r="B7" s="13"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="14"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="8">
+        <f>SUM(E2:E6)</f>
+        <v>1</v>
+      </c>
+      <c r="F8" s="18">
+        <f>SUM(F2:F6)</f>
+        <v>3.8949000000000004E-2</v>
+      </c>
+      <c r="G8" s="14"/>
+    </row>
+    <row r="10" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="13">
+        <v>18</v>
+      </c>
+      <c r="C11" s="3">
+        <f t="shared" ref="C11:C18" si="1">B11/AVG_CURRENT</f>
+        <v>462.14280212585686</v>
+      </c>
+      <c r="D11" s="15">
+        <f>C11/24</f>
+        <v>19.255950088577368</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="13">
+        <v>68</v>
+      </c>
+      <c r="C12" s="3">
+        <f t="shared" si="1"/>
+        <v>1745.8728080310148</v>
+      </c>
+      <c r="D12" s="15">
+        <f t="shared" ref="D12:D18" si="2">C12/24</f>
+        <v>72.74470033462562</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="20">
+        <v>210</v>
+      </c>
+      <c r="C13" s="21">
+        <f t="shared" si="1"/>
+        <v>5391.6660248016633</v>
+      </c>
+      <c r="D13" s="22">
+        <f t="shared" si="2"/>
+        <v>224.65275103340264</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="13">
+        <v>900</v>
+      </c>
+      <c r="C14" s="3">
+        <f t="shared" si="1"/>
+        <v>23107.140106292842</v>
+      </c>
+      <c r="D14" s="15">
+        <f t="shared" si="2"/>
+        <v>962.79750442886836</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" s="13">
+        <v>1250</v>
+      </c>
+      <c r="C15" s="3">
+        <f t="shared" si="1"/>
+        <v>32093.250147628947</v>
+      </c>
+      <c r="D15" s="15">
+        <f t="shared" si="2"/>
+        <v>1337.2187561512062</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" s="13">
+        <v>2400</v>
+      </c>
+      <c r="C16" s="3">
+        <f t="shared" si="1"/>
+        <v>61619.040283447575</v>
+      </c>
+      <c r="D16" s="15">
+        <f t="shared" si="2"/>
+        <v>2567.4600118103158</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" s="25">
+        <v>2890</v>
+      </c>
+      <c r="C17" s="26">
+        <f t="shared" si="1"/>
+        <v>74199.594341318123</v>
+      </c>
+      <c r="D17" s="27">
+        <f t="shared" si="2"/>
+        <v>3091.6497642215886</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18" s="14">
+        <v>4400</v>
+      </c>
+      <c r="C18" s="9">
+        <f t="shared" si="1"/>
+        <v>112968.24051965389</v>
+      </c>
+      <c r="D18" s="16">
+        <f t="shared" si="2"/>
+        <v>4707.0100216522451</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="46" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" s="15"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="13">
+        <v>0</v>
+      </c>
+      <c r="E2" s="5">
+        <v>0.9</v>
+      </c>
+      <c r="F2" s="17">
+        <f t="shared" ref="F2:F3" si="0">D2*E2</f>
+        <v>0</v>
+      </c>
+      <c r="G2" s="23" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="15"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="13">
+        <v>0.15</v>
+      </c>
+      <c r="E3" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="F3" s="17">
+        <f t="shared" si="0"/>
+        <v>1.5E-3</v>
+      </c>
+      <c r="G3" s="23" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="15"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="13">
+        <v>0.05</v>
+      </c>
+      <c r="E4" s="5">
+        <f>1-SUM(E2:E3)</f>
+        <v>8.9999999999999969E-2</v>
+      </c>
+      <c r="F4" s="17">
+        <f t="shared" ref="F4" si="1">D4*E4</f>
+        <v>4.4999999999999988E-3</v>
+      </c>
+      <c r="G4" s="23" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="2"/>
+      <c r="B5" s="13"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="13"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="14"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="8">
+        <f>SUM(E2:E3)</f>
+        <v>0.91</v>
+      </c>
+      <c r="F6" s="18">
+        <f>SUM(F2:F5)</f>
+        <v>5.9999999999999984E-3</v>
+      </c>
+      <c r="G6" s="14"/>
+    </row>
+    <row r="8" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="13">
+        <v>18</v>
+      </c>
+      <c r="C9" s="3">
+        <f t="shared" ref="C9:C16" si="2">B9/AVG_CURRENT</f>
+        <v>3000.0000000000009</v>
+      </c>
+      <c r="D9" s="15">
+        <f>C9/24</f>
+        <v>125.00000000000004</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="13">
+        <v>68</v>
+      </c>
+      <c r="C10" s="3">
+        <f t="shared" si="2"/>
+        <v>11333.333333333336</v>
+      </c>
+      <c r="D10" s="15">
+        <f t="shared" ref="D10:D16" si="3">C10/24</f>
+        <v>472.22222222222234</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="20">
+        <v>210</v>
+      </c>
+      <c r="C11" s="21">
+        <f t="shared" si="2"/>
+        <v>35000.000000000007</v>
+      </c>
+      <c r="D11" s="22">
+        <f t="shared" si="3"/>
+        <v>1458.3333333333337</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="13">
+        <v>900</v>
+      </c>
+      <c r="C12" s="3">
+        <f t="shared" si="2"/>
+        <v>150000.00000000003</v>
+      </c>
+      <c r="D12" s="15">
+        <f t="shared" si="3"/>
+        <v>6250.0000000000009</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="13">
+        <v>1250</v>
+      </c>
+      <c r="C13" s="3">
+        <f t="shared" si="2"/>
+        <v>208333.3333333334</v>
+      </c>
+      <c r="D13" s="15">
+        <f t="shared" si="3"/>
+        <v>8680.5555555555584</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="13">
+        <v>2400</v>
+      </c>
+      <c r="C14" s="3">
+        <f t="shared" si="2"/>
+        <v>400000.00000000012</v>
+      </c>
+      <c r="D14" s="15">
+        <f t="shared" si="3"/>
+        <v>16666.666666666672</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" s="25">
+        <v>2890</v>
+      </c>
+      <c r="C15" s="26">
+        <f t="shared" si="2"/>
+        <v>481666.6666666668</v>
+      </c>
+      <c r="D15" s="27">
+        <f t="shared" si="3"/>
+        <v>20069.444444444449</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" s="14">
+        <v>4400</v>
+      </c>
+      <c r="C16" s="9">
+        <f t="shared" si="2"/>
+        <v>733333.33333333349</v>
+      </c>
+      <c r="D16" s="16">
+        <f t="shared" si="3"/>
+        <v>30555.555555555562</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>